<commit_message>
adding cells with multilines (multicells)
</commit_message>
<xml_diff>
--- a/Apps/app4-invoice/invoices/10001-2023.1.18.xlsx
+++ b/Apps/app4-invoice/invoices/10001-2023.1.18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5de6fcc1d8554dbd/Desktop/Progetti/Corso Python/Apps/app4-invoice/invoices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_E74022ED2B5D1D142EC46EDD4B4427FC95C7990E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13CF53FE-A235-434F-970D-6F13C61C672A}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_E74022ED2B5D1D142EC46EDD4B4427FC95C7990E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93B1AC77-92D1-41AA-8195-D2ED516BC5CD}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="345" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
     <t>4772822</t>
   </si>
   <si>
-    <t>Microscope Landless Land</t>
+    <t>Microscope Landless Land fdghdsfyhsg</t>
   </si>
 </sst>
 </file>
@@ -341,6 +341,14 @@
 </file>
 
 <file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1425,7 +1433,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.9" customHeight="1"/>

</xml_diff>